<commit_message>
Multiple improvements: - fix #7 - url_builder method uses more pythonic syntax to format dates required in scraping url template - employed class variables to form dynamic csv file names dependant on url_builder output - performace_evaluation is no longer hardcoded and takes [self.] variables to read csv files and output - uploaded new sample files - deleted/ merged some comments.
</commit_message>
<xml_diff>
--- a/Performance.xlsx
+++ b/Performance.xlsx
@@ -24,34 +24,34 @@
     <t>Change, %</t>
   </si>
   <si>
+    <t>RAR1R</t>
+  </si>
+  <si>
+    <t>RKB1R</t>
+  </si>
+  <si>
+    <t>GRZ1R</t>
+  </si>
+  <si>
+    <t>AMG1L</t>
+  </si>
+  <si>
+    <t>LJM1R</t>
+  </si>
+  <si>
+    <t>SKN1T</t>
+  </si>
+  <si>
+    <t>MDARA</t>
+  </si>
+  <si>
+    <t>BAL1R</t>
+  </si>
+  <si>
     <t>GRD1R</t>
   </si>
   <si>
-    <t>LNS1L</t>
-  </si>
-  <si>
-    <t>VSS1R</t>
-  </si>
-  <si>
-    <t>SKN1T</t>
-  </si>
-  <si>
-    <t>TPD1T</t>
-  </si>
-  <si>
-    <t>RKB1R</t>
-  </si>
-  <si>
-    <t>GUB1L</t>
-  </si>
-  <si>
-    <t>UTR1L</t>
-  </si>
-  <si>
-    <t>LJM1R</t>
-  </si>
-  <si>
-    <t>KNR1L</t>
+    <t>HMX1R</t>
   </si>
 </sst>
 </file>
@@ -421,7 +421,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.06557377049180334</v>
+        <v>0.4563106796116503</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -429,7 +429,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0.04999999999999991</v>
+        <v>0.4492753623188405</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -437,7 +437,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.03333333333333337</v>
+        <v>0.3266666666666667</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -445,7 +445,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.03125000000000003</v>
+        <v>0.176470588235294</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -453,7 +453,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.02880658436213994</v>
+        <v>0.1444444444444445</v>
       </c>
     </row>
   </sheetData>
@@ -488,7 +488,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.2500000000000001</v>
+        <v>-0.08823529411764713</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -496,7 +496,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.1666666666666667</v>
+        <v>-0.06024096385542179</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -504,7 +504,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.1368421052631579</v>
+        <v>-0.05617977528089887</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -512,7 +512,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.1262135922330097</v>
+        <v>-0.01538461538461533</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -520,7 +520,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.08256880733944962</v>
+        <v>-0.007751937984496096</v>
       </c>
     </row>
   </sheetData>

</xml_diff>